<commit_message>
MAJOR TYPO FIXES GAAHH
</commit_message>
<xml_diff>
--- a/linreg/rifdid_coefs.xlsx
+++ b/linreg/rifdid_coefs.xlsx
@@ -582,16 +582,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.096230629600052561</v>
+        <v>-0.097464401122266106</v>
       </c>
       <c r="C2">
-        <v>0.0060584999520677061</v>
+        <v>0.0047164201965143402</v>
       </c>
       <c r="D2">
-        <v>-0.10810509418046191</v>
+        <v>-0.106708425304523</v>
       </c>
       <c r="E2">
-        <v>-0.084356165019643214</v>
+        <v>-0.088220376940009212</v>
       </c>
     </row>
     <row r="3">
@@ -599,16 +599,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-0.016450249925729826</v>
+        <v>-0.0056578454894290857</v>
       </c>
       <c r="C3">
-        <v>0.0074695073903815745</v>
+        <v>0.0065966016823923897</v>
       </c>
       <c r="D3">
-        <v>-0.031090243594446558</v>
+        <v>-0.018586961838692934</v>
       </c>
       <c r="E3">
-        <v>-0.0018102562570130962</v>
+        <v>0.007271270859834764</v>
       </c>
     </row>
     <row r="4">
@@ -616,16 +616,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-0.092744919408887516</v>
+        <v>-0.1159027882769664</v>
       </c>
       <c r="C4">
-        <v>0.0087744854461983633</v>
+        <v>0.0070461324870134999</v>
       </c>
       <c r="D4">
-        <v>-0.10994262799459774</v>
+        <v>-0.12971296981029889</v>
       </c>
       <c r="E4">
-        <v>-0.075547210823177294</v>
+        <v>-0.10209260674363391</v>
       </c>
     </row>
     <row r="5">
@@ -633,16 +633,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-0.03403305168786816</v>
+        <v>-0.031155157048010716</v>
       </c>
       <c r="C5">
-        <v>0.0038915456830830876</v>
+        <v>0.0027774659485927718</v>
       </c>
       <c r="D5">
-        <v>-0.041660355305894479</v>
+        <v>-0.036598896372993878</v>
       </c>
       <c r="E5">
-        <v>-0.026405748069841844</v>
+        <v>-0.025711417723027555</v>
       </c>
     </row>
     <row r="6">
@@ -650,16 +650,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.0037022922188086668</v>
+        <v>0.014602432614965579</v>
       </c>
       <c r="C6">
-        <v>0.0063260405797551092</v>
+        <v>0.0051147795200176989</v>
       </c>
       <c r="D6">
-        <v>-0.0086965426224466843</v>
+        <v>0.0045776377382377373</v>
       </c>
       <c r="E6">
-        <v>0.016101127060064016</v>
+        <v>0.02462722749169342</v>
       </c>
     </row>
     <row r="7">
@@ -667,16 +667,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>-0.074450386795289508</v>
+        <v>-0.078462762060216101</v>
       </c>
       <c r="C7">
-        <v>0.0058502020538126476</v>
+        <v>0.004337988310416434</v>
       </c>
       <c r="D7">
-        <v>-0.085916593522658277</v>
+        <v>-0.086965072437304933</v>
       </c>
       <c r="E7">
-        <v>-0.062984180067920739</v>
+        <v>-0.06996045168312727</v>
       </c>
     </row>
     <row r="8">
@@ -684,16 +684,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-0.1022722137770402</v>
+        <v>-0.10372393444060574</v>
       </c>
       <c r="C8">
-        <v>0.0069355137335835957</v>
+        <v>0.005633047677665497</v>
       </c>
       <c r="D8">
-        <v>-0.11586560184407214</v>
+        <v>-0.1147645202194586</v>
       </c>
       <c r="E8">
-        <v>-0.088678825710008249</v>
+        <v>-0.092683348661752873</v>
       </c>
     </row>
     <row r="9">
@@ -701,16 +701,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-0.015551599081443424</v>
+        <v>-0.00053886194556027013</v>
       </c>
       <c r="C9">
-        <v>0.0076817945026165504</v>
+        <v>0.006739010146725781</v>
       </c>
       <c r="D9">
-        <v>-0.030607673906819698</v>
+        <v>-0.013747097317770088</v>
       </c>
       <c r="E9">
-        <v>-0.00049552425606714905</v>
+        <v>0.012669373426649547</v>
       </c>
     </row>
     <row r="10">
@@ -718,16 +718,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-0.066518940939715776</v>
+        <v>-0.086265248758539123</v>
       </c>
       <c r="C10">
-        <v>0.0093412053589264857</v>
+        <v>0.0076870491642685159</v>
       </c>
       <c r="D10">
-        <v>-0.084827408680592992</v>
+        <v>-0.10133160902047431</v>
       </c>
       <c r="E10">
-        <v>-0.04821047319883856</v>
+        <v>-0.07119888849660394</v>
       </c>
     </row>
     <row r="11">
@@ -735,16 +735,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-0.042572030797728991</v>
+        <v>-0.03612250513490968</v>
       </c>
       <c r="C11">
-        <v>0.004380201709647767</v>
+        <v>0.0031748758867286659</v>
       </c>
       <c r="D11">
-        <v>-0.051157086962864404</v>
+        <v>-0.042345155677904006</v>
       </c>
       <c r="E11">
-        <v>-0.033986974632593578</v>
+        <v>-0.029899854591915354</v>
       </c>
     </row>
     <row r="12">
@@ -752,16 +752,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.0065394349344677473</v>
+        <v>0.017930200045447608</v>
       </c>
       <c r="C12">
-        <v>0.0064318040973285863</v>
+        <v>0.0051265806894197716</v>
       </c>
       <c r="D12">
-        <v>-0.0060666967185775888</v>
+        <v>0.0078822733708737887</v>
       </c>
       <c r="E12">
-        <v>0.019145566587513083</v>
+        <v>0.027978126720021427</v>
       </c>
     </row>
     <row r="13">
@@ -769,16 +769,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>-0.059674821632196638</v>
+        <v>-0.066068778449608373</v>
       </c>
       <c r="C13">
-        <v>0.0061430620955588971</v>
+        <v>0.0045830061966044468</v>
       </c>
       <c r="D13">
-        <v>-0.071715028136871181</v>
+        <v>-0.075051317300042594</v>
       </c>
       <c r="E13">
-        <v>-0.047634615127522095</v>
+        <v>-0.057086239599174159</v>
       </c>
     </row>
     <row r="14">
@@ -786,16 +786,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-0.20523053049203391</v>
+        <v>-0.21793794935324368</v>
       </c>
       <c r="C14">
-        <v>0.013769389276064579</v>
+        <v>0.0095995470310456278</v>
       </c>
       <c r="D14">
-        <v>-0.23221837655981833</v>
+        <v>-0.23675283617110043</v>
       </c>
       <c r="E14">
-        <v>-0.17824268442424948</v>
+        <v>-0.19912306253538692</v>
       </c>
     </row>
     <row r="15">
@@ -803,16 +803,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>-0.048887242948642044</v>
+        <v>-0.03490404981463039</v>
       </c>
       <c r="C15">
-        <v>0.021554675475050654</v>
+        <v>0.0188070857568692</v>
       </c>
       <c r="D15">
-        <v>-0.091134161246820528</v>
+        <v>-0.071765496375060106</v>
       </c>
       <c r="E15">
-        <v>-0.006640324650463568</v>
+        <v>0.0019573967457993252</v>
       </c>
     </row>
     <row r="16">
@@ -820,16 +820,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>-0.075206411090617334</v>
+        <v>-0.063714627108222704</v>
       </c>
       <c r="C16">
-        <v>0.026226187768748646</v>
+        <v>0.018957944579531049</v>
       </c>
       <c r="D16">
-        <v>-0.12660944024879156</v>
+        <v>-0.10087175341944465</v>
       </c>
       <c r="E16">
-        <v>-0.023803381932443107</v>
+        <v>-0.026557500797000762</v>
       </c>
     </row>
     <row r="17">
@@ -837,16 +837,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>-0.040559661012148203</v>
+        <v>-0.055731005675693106</v>
       </c>
       <c r="C17">
-        <v>0.011828710473158055</v>
+        <v>0.0081941477678990921</v>
       </c>
       <c r="D17">
-        <v>-0.063743823421833407</v>
+        <v>-0.071791365884865524</v>
       </c>
       <c r="E17">
-        <v>-0.017375498602463006</v>
+        <v>-0.039670645466520688</v>
       </c>
     </row>
     <row r="18">
@@ -854,16 +854,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.049059811339027544</v>
+        <v>0.023934697202849489</v>
       </c>
       <c r="C18">
-        <v>0.024517941672940101</v>
+        <v>0.020254325493546655</v>
       </c>
       <c r="D18">
-        <v>0.0010048739063699408</v>
+        <v>-0.015763362001614326</v>
       </c>
       <c r="E18">
-        <v>0.097114748771685147</v>
+        <v>0.063632756407313307</v>
       </c>
     </row>
     <row r="19">
@@ -871,16 +871,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>-0.086035231633252773</v>
+        <v>-0.091972688539959588</v>
       </c>
       <c r="C19">
-        <v>0.022414565021965562</v>
+        <v>0.01636262857585935</v>
       </c>
       <c r="D19">
-        <v>-0.12996757041108725</v>
+        <v>-0.12404310224749468</v>
       </c>
       <c r="E19">
-        <v>-0.042102892855418281</v>
+        <v>-0.059902274832424503</v>
       </c>
     </row>
     <row r="20">
@@ -888,16 +888,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>-0.16209551779232079</v>
+        <v>-0.1518914441128231</v>
       </c>
       <c r="C20">
-        <v>0.0060574416242696405</v>
+        <v>0.0045922904917993605</v>
       </c>
       <c r="D20">
-        <v>-0.17396790808436635</v>
+        <v>-0.16089217826910443</v>
       </c>
       <c r="E20">
-        <v>-0.15022312750027522</v>
+        <v>-0.14289070995654177</v>
       </c>
     </row>
     <row r="21">
@@ -905,16 +905,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>-0.022110569797575117</v>
+        <v>-0.018536542205195201</v>
       </c>
       <c r="C21">
-        <v>0.0076600676008701735</v>
+        <v>0.0065255551375708364</v>
       </c>
       <c r="D21">
-        <v>-0.037124055335200745</v>
+        <v>-0.031326409727799882</v>
       </c>
       <c r="E21">
-        <v>-0.0070970842599494908</v>
+        <v>-0.0057466746825905208</v>
       </c>
     </row>
     <row r="22">
@@ -922,16 +922,16 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>-0.10403823482689882</v>
+        <v>-0.11582145936915912</v>
       </c>
       <c r="C22">
-        <v>0.0086343202442496075</v>
+        <v>0.0067180479111650857</v>
       </c>
       <c r="D22">
-        <v>-0.12096122413570645</v>
+        <v>-0.12898860622224628</v>
       </c>
       <c r="E22">
-        <v>-0.087115245518091189</v>
+        <v>-0.10265431251607197</v>
       </c>
     </row>
     <row r="23">
@@ -939,16 +939,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>-0.060543757714499984</v>
+        <v>-0.046717381656622731</v>
       </c>
       <c r="C23">
-        <v>0.0039489228281133848</v>
+        <v>0.0028167454695602616</v>
       </c>
       <c r="D23">
-        <v>-0.06828351868020284</v>
+        <v>-0.052238107514263679</v>
       </c>
       <c r="E23">
-        <v>-0.052803996748797127</v>
+        <v>-0.041196655798981782</v>
       </c>
     </row>
     <row r="24">
@@ -956,16 +956,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>-0.019232451711013624</v>
+        <v>-0.0034584116232918723</v>
       </c>
       <c r="C24">
-        <v>0.0063181566991685756</v>
+        <v>0.0050916624774513617</v>
       </c>
       <c r="D24">
-        <v>-0.031615834401422294</v>
+        <v>-0.013437897878411072</v>
       </c>
       <c r="E24">
-        <v>-0.0068490690206049545</v>
+        <v>0.0065210746318273265</v>
       </c>
     </row>
     <row r="25">
@@ -973,16 +973,16 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>-0.088404668188360291</v>
+        <v>-0.093252739145536945</v>
       </c>
       <c r="C25">
-        <v>0.0057082410987553973</v>
+        <v>0.0042102482783304774</v>
       </c>
       <c r="D25">
-        <v>-0.099592636037323087</v>
+        <v>-0.10150468337992176</v>
       </c>
       <c r="E25">
-        <v>-0.077216700339397495</v>
+        <v>-0.08500079491115213</v>
       </c>
     </row>
     <row r="26">
@@ -990,16 +990,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>-0.17477589458865286</v>
+        <v>-0.16138422137269409</v>
       </c>
       <c r="C26">
-        <v>0.0070308012111219217</v>
+        <v>0.0053216936791763599</v>
       </c>
       <c r="D26">
-        <v>-0.18855604310485455</v>
+        <v>-0.17181456368750925</v>
       </c>
       <c r="E26">
-        <v>-0.16099574607245118</v>
+        <v>-0.15095387905787894</v>
       </c>
     </row>
     <row r="27">
@@ -1007,16 +1007,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>-0.012483844008956229</v>
+        <v>-0.0053036443585133828</v>
       </c>
       <c r="C27">
-        <v>0.0080059464071029172</v>
+        <v>0.0065163525964822815</v>
       </c>
       <c r="D27">
-        <v>-0.028175246338481775</v>
+        <v>-0.018075478350255678</v>
       </c>
       <c r="E27">
-        <v>0.0032075583205693169</v>
+        <v>0.0074681896332289112</v>
       </c>
     </row>
     <row r="28">
@@ -1024,16 +1024,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>-0.073156702488253303</v>
+        <v>-0.077952273634404337</v>
       </c>
       <c r="C28">
-        <v>0.0094163166639254468</v>
+        <v>0.007193270864007951</v>
       </c>
       <c r="D28">
-        <v>-0.091612386016784148</v>
+        <v>-0.092050844878437538</v>
       </c>
       <c r="E28">
-        <v>-0.054701018959722458</v>
+        <v>-0.063853702390371136</v>
       </c>
     </row>
     <row r="29">
@@ -1041,16 +1041,16 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>-0.067378506761092638</v>
+        <v>-0.055444443251652917</v>
       </c>
       <c r="C29">
-        <v>0.0043108027564700791</v>
+        <v>0.00315632910421216</v>
       </c>
       <c r="D29">
-        <v>-0.075827543183228596</v>
+        <v>-0.061630742721277866</v>
       </c>
       <c r="E29">
-        <v>-0.058929470338956673</v>
+        <v>-0.049258143782027967</v>
       </c>
     </row>
     <row r="30">
@@ -1058,16 +1058,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>-0.019007153156826228</v>
+        <v>0.0024240933039623527</v>
       </c>
       <c r="C30">
-        <v>0.0062752524914340274</v>
+        <v>0.0050776058121814131</v>
       </c>
       <c r="D30">
-        <v>-0.031306448636919379</v>
+        <v>-0.0075278442493628989</v>
       </c>
       <c r="E30">
-        <v>-0.0067078576767330752</v>
+        <v>0.012376030857287603</v>
       </c>
     </row>
     <row r="31">
@@ -1075,16 +1075,16 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>-0.070562357658617042</v>
+        <v>-0.075627684242248611</v>
       </c>
       <c r="C31">
-        <v>0.0058915229198202128</v>
+        <v>0.0044160198464212276</v>
       </c>
       <c r="D31">
-        <v>-0.082109555371780441</v>
+        <v>-0.084282935431774952</v>
       </c>
       <c r="E31">
-        <v>-0.059015159945453637</v>
+        <v>-0.066972433052722269</v>
       </c>
     </row>
     <row r="32">
@@ -1092,16 +1092,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>-0.18371156936993338</v>
+        <v>-0.17647299717056505</v>
       </c>
       <c r="C32">
-        <v>0.0096919523640901385</v>
+        <v>0.0065354713109747357</v>
       </c>
       <c r="D32">
-        <v>-0.20270768555593183</v>
+        <v>-0.18928236751060973</v>
       </c>
       <c r="E32">
-        <v>-0.16471545318393493</v>
+        <v>-0.16366362683052038</v>
       </c>
     </row>
     <row r="33">
@@ -1109,16 +1109,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>-0.035654335361604686</v>
+        <v>-0.043925165953804989</v>
       </c>
       <c r="C33">
-        <v>0.017150051678373586</v>
+        <v>0.014198734369485076</v>
       </c>
       <c r="D33">
-        <v>-0.069268241212538634</v>
+        <v>-0.071754351982551978</v>
       </c>
       <c r="E33">
-        <v>-0.0020404295106707451</v>
+        <v>-0.016095979925057999</v>
       </c>
     </row>
     <row r="34">
@@ -1126,16 +1126,16 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>-0.056481389999193679</v>
+        <v>-0.060598094666297224</v>
       </c>
       <c r="C34">
-        <v>0.018248324652956095</v>
+        <v>0.012684182232458216</v>
       </c>
       <c r="D34">
-        <v>-0.092247898364602537</v>
+        <v>-0.085458794062732824</v>
       </c>
       <c r="E34">
-        <v>-0.020714881633784828</v>
+        <v>-0.035737395269861624</v>
       </c>
     </row>
     <row r="35">
@@ -1143,16 +1143,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>-0.053062633575798192</v>
+        <v>-0.04625215340262797</v>
       </c>
       <c r="C35">
-        <v>0.0087418726019109563</v>
+        <v>0.0060791090910996097</v>
       </c>
       <c r="D35">
-        <v>-0.070196622494318989</v>
+        <v>-0.058167081534189674</v>
       </c>
       <c r="E35">
-        <v>-0.035928644657277402</v>
+        <v>-0.034337225271066266</v>
       </c>
     </row>
     <row r="36">
@@ -1160,16 +1160,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>0.0099297612965005364</v>
+        <v>0.0056337196904819387</v>
       </c>
       <c r="C36">
-        <v>0.019235265588138751</v>
+        <v>0.015932426772457493</v>
       </c>
       <c r="D36">
-        <v>-0.027771180188271134</v>
+        <v>-0.025593507376907791</v>
       </c>
       <c r="E36">
-        <v>0.047630702781272204</v>
+        <v>0.036860946757871667</v>
       </c>
     </row>
     <row r="37">
@@ -1177,16 +1177,16 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>-0.071171235753681991</v>
+        <v>-0.083611813585319647</v>
       </c>
       <c r="C37">
-        <v>0.01627090315103219</v>
+        <v>0.011698069247767028</v>
       </c>
       <c r="D37">
-        <v>-0.10306205445803701</v>
+        <v>-0.10653978745064215</v>
       </c>
       <c r="E37">
-        <v>-0.039280417049326978</v>
+        <v>-0.060683839719997149</v>
       </c>
     </row>
     <row r="38">
@@ -1194,16 +1194,16 @@
         <v>41</v>
       </c>
       <c r="B38">
-        <v>-0.18805656295856696</v>
+        <v>-0.1689285355750734</v>
       </c>
       <c r="C38">
-        <v>0.005338084382884186</v>
+        <v>0.0040344313131793399</v>
       </c>
       <c r="D38">
-        <v>-0.19851903624952758</v>
+        <v>-0.17683588459546953</v>
       </c>
       <c r="E38">
-        <v>-0.17759408966760634</v>
+        <v>-0.16102118655467726</v>
       </c>
     </row>
     <row r="39">
@@ -1211,16 +1211,16 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>-0.02384220259384133</v>
+        <v>-0.02796874346919705</v>
       </c>
       <c r="C39">
-        <v>0.0070578179707198874</v>
+        <v>0.0059487543699251761</v>
       </c>
       <c r="D39">
-        <v>-0.037675298272861195</v>
+        <v>-0.039628100981603444</v>
       </c>
       <c r="E39">
-        <v>-0.010009106914821464</v>
+        <v>-0.016309385956790656</v>
       </c>
     </row>
     <row r="40">
@@ -1228,16 +1228,16 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>-0.079572187261448171</v>
+        <v>-0.087828573633573701</v>
       </c>
       <c r="C40">
-        <v>0.0074407913862621997</v>
+        <v>0.0057553798795320797</v>
       </c>
       <c r="D40">
-        <v>-0.094155898487893033</v>
+        <v>-0.099108923680371649</v>
       </c>
       <c r="E40">
-        <v>-0.064988476035003309</v>
+        <v>-0.076548223586775752</v>
       </c>
     </row>
     <row r="41">
@@ -1245,16 +1245,16 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>-0.084337151400070823</v>
+        <v>-0.06265905050083645</v>
       </c>
       <c r="C41">
-        <v>0.004004842491271257</v>
+        <v>0.0029127658436635009</v>
       </c>
       <c r="D41">
-        <v>-0.092186513096140787</v>
+        <v>-0.068367973044298244</v>
       </c>
       <c r="E41">
-        <v>-0.076487789704000858</v>
+        <v>-0.056950127957374662</v>
       </c>
     </row>
     <row r="42">
@@ -1262,16 +1262,16 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>-0.016448827262993251</v>
+        <v>-0.001441719185437004</v>
       </c>
       <c r="C42">
-        <v>0.0064048032301471935</v>
+        <v>0.0052142785293559394</v>
       </c>
       <c r="D42">
-        <v>-0.029002034350452056</v>
+        <v>-0.011661528755398394</v>
       </c>
       <c r="E42">
-        <v>-0.003895620175534447</v>
+        <v>0.0087780903845243868</v>
       </c>
     </row>
     <row r="43">
@@ -1279,16 +1279,16 @@
         <v>46</v>
       </c>
       <c r="B43">
-        <v>-0.073948548480878479</v>
+        <v>-0.086932951332555575</v>
       </c>
       <c r="C43">
-        <v>0.0056134829344718952</v>
+        <v>0.0042029447660548742</v>
       </c>
       <c r="D43">
-        <v>-0.084950793393986007</v>
+        <v>-0.095170580929885937</v>
       </c>
       <c r="E43">
-        <v>-0.06294630356777095</v>
+        <v>-0.078695321735225213</v>
       </c>
     </row>
     <row r="44">
@@ -1296,16 +1296,16 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>-0.208898916445759</v>
+        <v>-0.182504756141942</v>
       </c>
       <c r="C44">
-        <v>0.0062606166181625516</v>
+        <v>0.0047709045476295462</v>
       </c>
       <c r="D44">
-        <v>-0.22116952746300803</v>
+        <v>-0.1918555701088944</v>
       </c>
       <c r="E44">
-        <v>-0.19662830542850998</v>
+        <v>-0.17315394217498961</v>
       </c>
     </row>
     <row r="45">
@@ -1313,16 +1313,16 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>-0.014870219837446345</v>
+        <v>-0.0084503315535184153</v>
       </c>
       <c r="C45">
-        <v>0.007538488429631964</v>
+        <v>0.0061873988611498877</v>
       </c>
       <c r="D45">
-        <v>-0.029645419281809519</v>
+        <v>-0.020577427183359163</v>
       </c>
       <c r="E45">
-        <v>-9.502039308316966e-05</v>
+        <v>0.0036767640763223346</v>
       </c>
     </row>
     <row r="46">
@@ -1330,16 +1330,16 @@
         <v>49</v>
       </c>
       <c r="B46">
-        <v>-0.04829621531353543</v>
+        <v>-0.062048066975736248</v>
       </c>
       <c r="C46">
-        <v>0.0082915730349090999</v>
+        <v>0.0063829091868396696</v>
       </c>
       <c r="D46">
-        <v>-0.064547436820585835</v>
+        <v>-0.07455835633035017</v>
       </c>
       <c r="E46">
-        <v>-0.032044993806485025</v>
+        <v>-0.049537777621122325</v>
       </c>
     </row>
     <row r="47">
@@ -1347,16 +1347,16 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <v>-0.099236520273736459</v>
+        <v>-0.078568813516409444</v>
       </c>
       <c r="C47">
-        <v>0.0044719456568046816</v>
+        <v>0.003285452402462976</v>
       </c>
       <c r="D47">
-        <v>-0.10800139166003361</v>
+        <v>-0.085008190331618938</v>
       </c>
       <c r="E47">
-        <v>-0.090471648887439304</v>
+        <v>-0.07212943670119995</v>
       </c>
     </row>
     <row r="48">
@@ -1364,16 +1364,16 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>-0.015764020095112664</v>
+        <v>0.00027269526650030678</v>
       </c>
       <c r="C48">
-        <v>0.0065602073203329088</v>
+        <v>0.0052580906070533217</v>
       </c>
       <c r="D48">
-        <v>-0.028621817985091454</v>
+        <v>-0.010032986447819256</v>
       </c>
       <c r="E48">
-        <v>-0.0029062222051338769</v>
+        <v>0.010578376980819868</v>
       </c>
     </row>
     <row r="49">
@@ -1381,16 +1381,16 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>-0.06166051438865762</v>
+        <v>-0.069518524702940163</v>
       </c>
       <c r="C49">
-        <v>0.0059812970367568372</v>
+        <v>0.0044814480265952823</v>
       </c>
       <c r="D49">
-        <v>-0.073383666518344534</v>
+        <v>-0.078302012937129906</v>
       </c>
       <c r="E49">
-        <v>-0.049937362258970705</v>
+        <v>-0.060735036468750413</v>
       </c>
     </row>
     <row r="50">
@@ -1398,16 +1398,16 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>-0.16504874490108565</v>
+        <v>-0.15409006833229191</v>
       </c>
       <c r="C50">
-        <v>0.0081199788634559907</v>
+        <v>0.0055054226019856864</v>
       </c>
       <c r="D50">
-        <v>-0.18096381093974773</v>
+        <v>-0.1648805673845736</v>
       </c>
       <c r="E50">
-        <v>-0.14913367886242357</v>
+        <v>-0.14329956928001022</v>
       </c>
     </row>
     <row r="51">
@@ -1415,16 +1415,16 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>-0.040085656931958327</v>
+        <v>-0.046967359615533798</v>
       </c>
       <c r="C51">
-        <v>0.014871991782758746</v>
+        <v>0.01237113719617973</v>
       </c>
       <c r="D51">
-        <v>-0.069234591347817995</v>
+        <v>-0.071214498090040143</v>
       </c>
       <c r="E51">
-        <v>-0.010936722516098656</v>
+        <v>-0.022720221141027456</v>
       </c>
     </row>
     <row r="52">
@@ -1432,16 +1432,16 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>-0.032552360777065102</v>
+        <v>-0.038767680181503082</v>
       </c>
       <c r="C52">
-        <v>0.014919239122117898</v>
+        <v>0.010407272092574991</v>
       </c>
       <c r="D52">
-        <v>-0.061793899439647151</v>
+        <v>-0.059165689157465062</v>
       </c>
       <c r="E52">
-        <v>-0.003310822114483053</v>
+        <v>-0.018369671205541106</v>
       </c>
     </row>
     <row r="53">
@@ -1449,16 +1449,16 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>-0.062779713555566274</v>
+        <v>-0.047403832827668635</v>
       </c>
       <c r="C53">
-        <v>0.0077015141078564447</v>
+        <v>0.0055064572313329417</v>
       </c>
       <c r="D53">
-        <v>-0.077874609510810253</v>
+        <v>-0.058196375153797983</v>
       </c>
       <c r="E53">
-        <v>-0.047684817600322296</v>
+        <v>-0.036611290501539287</v>
       </c>
     </row>
     <row r="54">
@@ -1466,16 +1466,16 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>-0.023338743328945352</v>
+        <v>-0.015073418754080381</v>
       </c>
       <c r="C54">
-        <v>0.017189361763643524</v>
+        <v>0.014740268974442493</v>
       </c>
       <c r="D54">
-        <v>-0.057029732363758225</v>
+        <v>-0.043964041185500298</v>
       </c>
       <c r="E54">
-        <v>0.01035224570586752</v>
+        <v>0.013817203677339534</v>
       </c>
     </row>
     <row r="55">
@@ -1483,16 +1483,16 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>-0.026400952493695957</v>
+        <v>-0.05302666632747368</v>
       </c>
       <c r="C55">
-        <v>0.014273407115673636</v>
+        <v>0.010407923284904074</v>
       </c>
       <c r="D55">
-        <v>-0.054376697564154593</v>
+        <v>-0.073425980779652456</v>
       </c>
       <c r="E55">
-        <v>0.0015747925767626778</v>
+        <v>-0.032627351875294898</v>
       </c>
     </row>
     <row r="56">
@@ -1500,16 +1500,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>-0.1930479574395968</v>
+        <v>-0.16984529737892404</v>
       </c>
       <c r="C56">
-        <v>0.0048911470346848533</v>
+        <v>0.0036618642533737806</v>
       </c>
       <c r="D56">
-        <v>-0.20263444793731766</v>
+        <v>-0.17702242755391276</v>
       </c>
       <c r="E56">
-        <v>-0.18346146694187593</v>
+        <v>-0.16266816720393532</v>
       </c>
     </row>
     <row r="57">
@@ -1517,16 +1517,16 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>-0.032447356752610755</v>
+        <v>-0.041042283135822047</v>
       </c>
       <c r="C57">
-        <v>0.0067404512176433935</v>
+        <v>0.0056164824188114151</v>
       </c>
       <c r="D57">
-        <v>-0.045658423827484113</v>
+        <v>-0.052050398853985574</v>
       </c>
       <c r="E57">
-        <v>-0.019236289677737394</v>
+        <v>-0.030034167417658519</v>
       </c>
     </row>
     <row r="58">
@@ -1534,16 +1534,16 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>-0.048460202689778908</v>
+        <v>-0.04740374953744024</v>
       </c>
       <c r="C58">
-        <v>0.0066772095533564326</v>
+        <v>0.0050933223052788464</v>
       </c>
       <c r="D58">
-        <v>-0.061547318141556957</v>
+        <v>-0.057386489114550548</v>
       </c>
       <c r="E58">
-        <v>-0.03537308723800086</v>
+        <v>-0.037421009960329932</v>
       </c>
     </row>
     <row r="59">
@@ -1551,16 +1551,16 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>-0.094481639590762681</v>
+        <v>-0.072034393370609101</v>
       </c>
       <c r="C59">
-        <v>0.0038280014601334835</v>
+        <v>0.0028207215861316692</v>
       </c>
       <c r="D59">
-        <v>-0.10198439858794205</v>
+        <v>-0.077562912282257229</v>
       </c>
       <c r="E59">
-        <v>-0.086978880593583316</v>
+        <v>-0.066505874458960973</v>
       </c>
     </row>
     <row r="60">
@@ -1568,16 +1568,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>-0.020339196969260988</v>
+        <v>-0.010920054360333026</v>
       </c>
       <c r="C60">
-        <v>0.0061833254398118388</v>
+        <v>0.005071012140768179</v>
       </c>
       <c r="D60">
-        <v>-0.032458314754137331</v>
+        <v>-0.020859066653950251</v>
       </c>
       <c r="E60">
-        <v>-0.0082200791843846446</v>
+        <v>-0.00098104206671579923</v>
       </c>
     </row>
     <row r="61">
@@ -1585,16 +1585,16 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>-0.057995913270445329</v>
+        <v>-0.070044560373682466</v>
       </c>
       <c r="C61">
-        <v>0.0052714581410322004</v>
+        <v>0.0039769903389954486</v>
       </c>
       <c r="D61">
-        <v>-0.068327800655489476</v>
+        <v>-0.077839326935784395</v>
       </c>
       <c r="E61">
-        <v>-0.047664025885401175</v>
+        <v>-0.062249793811580537</v>
       </c>
     </row>
     <row r="62">
@@ -1602,16 +1602,16 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>-0.22094656641135108</v>
+        <v>-0.18700037302294645</v>
       </c>
       <c r="C62">
-        <v>0.0058177952725946046</v>
+        <v>0.0043903812058257961</v>
       </c>
       <c r="D62">
-        <v>-0.23234926156455635</v>
+        <v>-0.19560537391739505</v>
       </c>
       <c r="E62">
-        <v>-0.2095438712581458</v>
+        <v>-0.17839537212849785</v>
       </c>
     </row>
     <row r="63">
@@ -1619,16 +1619,16 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>-0.026959703248176307</v>
+        <v>-0.025503480936862995</v>
       </c>
       <c r="C63">
-        <v>0.007429461060728287</v>
+        <v>0.0060169957569033896</v>
       </c>
       <c r="D63">
-        <v>-0.041521212489857212</v>
+        <v>-0.03729659215949277</v>
       </c>
       <c r="E63">
-        <v>-0.012398194006495401</v>
+        <v>-0.013710369714233221</v>
       </c>
     </row>
     <row r="64">
@@ -1636,16 +1636,16 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>-0.022134761603659747</v>
+        <v>-0.03225612251669463</v>
       </c>
       <c r="C64">
-        <v>0.0076224461251837962</v>
+        <v>0.0057984864412830911</v>
       </c>
       <c r="D64">
-        <v>-0.037074515482011489</v>
+        <v>-0.043620962760516691</v>
       </c>
       <c r="E64">
-        <v>-0.0071950077253080044</v>
+        <v>-0.020891282272872572</v>
       </c>
     </row>
     <row r="65">
@@ -1653,16 +1653,16 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>-0.11827111975234035</v>
+        <v>-0.095310901832793962</v>
       </c>
       <c r="C65">
-        <v>0.004322221568008348</v>
+        <v>0.003245014334796935</v>
       </c>
       <c r="D65">
-        <v>-0.12674253668224592</v>
+        <v>-0.10167102138797274</v>
       </c>
       <c r="E65">
-        <v>-0.1097997028224348</v>
+        <v>-0.088950782277615187</v>
       </c>
     </row>
     <row r="66">
@@ -1670,16 +1670,16 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>-0.019194210877435662</v>
+        <v>-0.0032849139735790897</v>
       </c>
       <c r="C66">
-        <v>0.0064819900041010086</v>
+        <v>0.0052515324388209489</v>
       </c>
       <c r="D66">
-        <v>-0.031898705313042022</v>
+        <v>-0.013577741897524417</v>
       </c>
       <c r="E66">
-        <v>-0.0064897164418293036</v>
+        <v>0.0070079139503662381</v>
       </c>
     </row>
     <row r="67">
@@ -1687,16 +1687,16 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>-0.038831117428064853</v>
+        <v>-0.048212500962544161</v>
       </c>
       <c r="C67">
-        <v>0.005720969085501632</v>
+        <v>0.0043556227242508476</v>
       </c>
       <c r="D67">
-        <v>-0.050044035045501353</v>
+        <v>-0.056749375812812697</v>
       </c>
       <c r="E67">
-        <v>-0.027618199810628352</v>
+        <v>-0.039675626112275625</v>
       </c>
     </row>
     <row r="68">
@@ -1704,16 +1704,16 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>-0.14941618365292483</v>
+        <v>-0.13387785084215059</v>
       </c>
       <c r="C68">
-        <v>0.0071166629990078584</v>
+        <v>0.0049186565356400744</v>
       </c>
       <c r="D68">
-        <v>-0.1633647620308625</v>
+        <v>-0.14351830217956116</v>
       </c>
       <c r="E68">
-        <v>-0.13546760527498716</v>
+        <v>-0.12423739950474003</v>
       </c>
     </row>
     <row r="69">
@@ -1721,16 +1721,16 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>-0.043875222356360731</v>
+        <v>-0.046719681680247357</v>
       </c>
       <c r="C69">
-        <v>0.013278524652985669</v>
+        <v>0.011266615859847067</v>
       </c>
       <c r="D69">
-        <v>-0.06990097935670897</v>
+        <v>-0.068801984265747865</v>
       </c>
       <c r="E69">
-        <v>-0.017849465356012485</v>
+        <v>-0.024637379094746847</v>
       </c>
     </row>
     <row r="70">
@@ -1738,16 +1738,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>-0.017750133857604215</v>
+        <v>-0.030370289682911764</v>
       </c>
       <c r="C70">
-        <v>0.012785040119354548</v>
+        <v>0.009055046719176443</v>
       </c>
       <c r="D70">
-        <v>-0.042808666795689954</v>
+        <v>-0.048117968672422642</v>
       </c>
       <c r="E70">
-        <v>0.0073083990804815209</v>
+        <v>-0.012622610693400881</v>
       </c>
     </row>
     <row r="71">
@@ -1755,16 +1755,16 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>-0.06576507801533539</v>
+        <v>-0.046895695285811279</v>
       </c>
       <c r="C71">
-        <v>0.0069316783207947529</v>
+        <v>0.0050075186225841135</v>
       </c>
       <c r="D71">
-        <v>-0.07935110299461566</v>
+        <v>-0.056710328254464634</v>
       </c>
       <c r="E71">
-        <v>-0.05217905303605512</v>
+        <v>-0.037081062317157923</v>
       </c>
     </row>
     <row r="72">
@@ -1772,16 +1772,16 @@
         <v>75</v>
       </c>
       <c r="B72">
-        <v>-0.036497590048388588</v>
+        <v>-0.047338143886766701</v>
       </c>
       <c r="C72">
-        <v>0.015275453316505306</v>
+        <v>0.013468500755953251</v>
       </c>
       <c r="D72">
-        <v>-0.066437336344070133</v>
+        <v>-0.073736126904051236</v>
       </c>
       <c r="E72">
-        <v>-0.0065578437527070432</v>
+        <v>-0.020940160869482166</v>
       </c>
     </row>
     <row r="73">
@@ -1789,16 +1789,16 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>0.009281143814386484</v>
+        <v>-0.021536995637974926</v>
       </c>
       <c r="C73">
-        <v>0.012834900659709927</v>
+        <v>0.0094992381084423889</v>
       </c>
       <c r="D73">
-        <v>-0.015875141993955368</v>
+        <v>-0.040155305931566049</v>
       </c>
       <c r="E73">
-        <v>0.034437429622728333</v>
+        <v>-0.0029186853443838</v>
       </c>
     </row>
     <row r="74">
@@ -1806,16 +1806,16 @@
         <v>77</v>
       </c>
       <c r="B74">
-        <v>-0.19216861456401232</v>
+        <v>-0.16132455495823389</v>
       </c>
       <c r="C74">
-        <v>0.0047366958018826844</v>
+        <v>0.0034825248211786505</v>
       </c>
       <c r="D74">
-        <v>-0.20145238562493864</v>
+        <v>-0.16815018590733319</v>
       </c>
       <c r="E74">
-        <v>-0.18288484350308601</v>
+        <v>-0.15449892400913459</v>
       </c>
     </row>
     <row r="75">
@@ -1823,16 +1823,16 @@
         <v>78</v>
       </c>
       <c r="B75">
-        <v>-0.033788148196011815</v>
+        <v>-0.048651046734607802</v>
       </c>
       <c r="C75">
-        <v>0.0066730068865615329</v>
+        <v>0.0054513335657894839</v>
       </c>
       <c r="D75">
-        <v>-0.046867026556365564</v>
+        <v>-0.059335476282456188</v>
       </c>
       <c r="E75">
-        <v>-0.020709269835658066</v>
+        <v>-0.037966617186759415</v>
       </c>
     </row>
     <row r="76">
@@ -1840,16 +1840,16 @@
         <v>79</v>
       </c>
       <c r="B76">
-        <v>-0.019876500016158677</v>
+        <v>-0.020900014724883054</v>
       </c>
       <c r="C76">
-        <v>0.0063332767066470418</v>
+        <v>0.0047244269601169524</v>
       </c>
       <c r="D76">
-        <v>-0.032289518176758868</v>
+        <v>-0.030159731893192987</v>
       </c>
       <c r="E76">
-        <v>-0.0074634818555584844</v>
+        <v>-0.011640297556573122</v>
       </c>
     </row>
     <row r="77">
@@ -1857,16 +1857,16 @@
         <v>80</v>
       </c>
       <c r="B77">
-        <v>-0.10146889932996572</v>
+        <v>-0.076284748435595615</v>
       </c>
       <c r="C77">
-        <v>0.003955244831894301</v>
+        <v>0.0028741810673170187</v>
       </c>
       <c r="D77">
-        <v>-0.10922105121851473</v>
+        <v>-0.081918046122360436</v>
       </c>
       <c r="E77">
-        <v>-0.093716747441416712</v>
+        <v>-0.070651450748830794</v>
       </c>
     </row>
     <row r="78">
@@ -1874,16 +1874,16 @@
         <v>81</v>
       </c>
       <c r="B78">
-        <v>-0.031346314473694591</v>
+        <v>-0.027656639201852521</v>
       </c>
       <c r="C78">
-        <v>0.0063466550977532704</v>
+        <v>0.0051339522989187168</v>
       </c>
       <c r="D78">
-        <v>-0.043785553103191398</v>
+        <v>-0.037719012076800493</v>
       </c>
       <c r="E78">
-        <v>-0.018907075844197783</v>
+        <v>-0.017594266326904553</v>
       </c>
     </row>
     <row r="79">
@@ -1891,16 +1891,16 @@
         <v>82</v>
       </c>
       <c r="B79">
-        <v>-0.045224968999124641</v>
+        <v>-0.056593316699201243</v>
       </c>
       <c r="C79">
-        <v>0.0053426779138432377</v>
+        <v>0.0039676874044034839</v>
       </c>
       <c r="D79">
-        <v>-0.055696444834382304</v>
+        <v>-0.064369849824129369</v>
       </c>
       <c r="E79">
-        <v>-0.034753493163866979</v>
+        <v>-0.048816783574273111</v>
       </c>
     </row>
     <row r="80">
@@ -1908,16 +1908,16 @@
         <v>83</v>
       </c>
       <c r="B80">
-        <v>-0.21064301185786727</v>
+        <v>-0.1864259614496119</v>
       </c>
       <c r="C80">
-        <v>0.0054477694438792379</v>
+        <v>0.0042484230904590858</v>
       </c>
       <c r="D80">
-        <v>-0.22132046806299047</v>
+        <v>-0.19475272916738695</v>
       </c>
       <c r="E80">
-        <v>-0.19996555565274407</v>
+        <v>-0.17809919373183686</v>
       </c>
     </row>
     <row r="81">
@@ -1925,16 +1925,16 @@
         <v>84</v>
       </c>
       <c r="B81">
-        <v>-0.027240063567160151</v>
+        <v>-0.029912055224092855</v>
       </c>
       <c r="C81">
-        <v>0.0072743101124160044</v>
+        <v>0.0061136704105074638</v>
       </c>
       <c r="D81">
-        <v>-0.041497481845951832</v>
+        <v>-0.041894645546995221</v>
       </c>
       <c r="E81">
-        <v>-0.012982645288368467</v>
+        <v>-0.017929464901190489</v>
       </c>
     </row>
     <row r="82">
@@ -1942,16 +1942,16 @@
         <v>85</v>
       </c>
       <c r="B82">
-        <v>-0.0066917558216110186</v>
+        <v>-0.0090248630092466808</v>
       </c>
       <c r="C82">
-        <v>0.0070702120842819896</v>
+        <v>0.0055420351937933649</v>
       </c>
       <c r="D82">
-        <v>-0.020549148405592615</v>
+        <v>-0.019887067351861961</v>
       </c>
       <c r="E82">
-        <v>0.0071656367623705785</v>
+        <v>0.0018373413333685994</v>
       </c>
     </row>
     <row r="83">
@@ -1959,16 +1959,16 @@
         <v>86</v>
       </c>
       <c r="B83">
-        <v>-0.12437306486036999</v>
+        <v>-0.10523665291054156</v>
       </c>
       <c r="C83">
-        <v>0.0043682463360932618</v>
+        <v>0.0033222608675551857</v>
       </c>
       <c r="D83">
-        <v>-0.13293468887323384</v>
+        <v>-0.111748173086142</v>
       </c>
       <c r="E83">
-        <v>-0.11581144084750614</v>
+        <v>-0.098725132734941115</v>
       </c>
     </row>
     <row r="84">
@@ -1976,16 +1976,16 @@
         <v>87</v>
       </c>
       <c r="B84">
-        <v>-0.028970313346106356</v>
+        <v>-0.01909554944164648</v>
       </c>
       <c r="C84">
-        <v>0.0065755448531309652</v>
+        <v>0.0054597057405839436</v>
       </c>
       <c r="D84">
-        <v>-0.041858172313002193</v>
+        <v>-0.029796390073952246</v>
       </c>
       <c r="E84">
-        <v>-0.01608245437921052</v>
+        <v>-0.0083947088093407115</v>
       </c>
     </row>
     <row r="85">
@@ -1993,16 +1993,16 @@
         <v>88</v>
       </c>
       <c r="B85">
-        <v>-0.030010174317494216</v>
+        <v>-0.038424556586530621</v>
       </c>
       <c r="C85">
-        <v>0.0057051769161376668</v>
+        <v>0.0044117204117669478</v>
       </c>
       <c r="D85">
-        <v>-0.041192139784791061</v>
+        <v>-0.047071381027944427</v>
       </c>
       <c r="E85">
-        <v>-0.01882820885019737</v>
+        <v>-0.029777732145116816</v>
       </c>
     </row>
     <row r="86">
@@ -2010,16 +2010,16 @@
         <v>89</v>
       </c>
       <c r="B86">
-        <v>-0.13162406223811113</v>
+        <v>-0.11787290418496947</v>
       </c>
       <c r="C86">
-        <v>0.0065795484241408008</v>
+        <v>0.0043647094039408769</v>
       </c>
       <c r="D86">
-        <v>-0.14451990217016336</v>
+        <v>-0.12642763214894484</v>
       </c>
       <c r="E86">
-        <v>-0.11872822230605888</v>
+        <v>-0.10931817622099411</v>
       </c>
     </row>
     <row r="87">
@@ -2027,16 +2027,16 @@
         <v>90</v>
       </c>
       <c r="B87">
-        <v>-0.052422586829301024</v>
+        <v>-0.059952633936656827</v>
       </c>
       <c r="C87">
-        <v>0.012235162529242475</v>
+        <v>0.010093456089698548</v>
       </c>
       <c r="D87">
-        <v>-0.076403365957065969</v>
+        <v>-0.079735570914257092</v>
       </c>
       <c r="E87">
-        <v>-0.028441807701536082</v>
+        <v>-0.040169696959056561</v>
       </c>
     </row>
     <row r="88">
@@ -2044,16 +2044,16 @@
         <v>91</v>
       </c>
       <c r="B88">
-        <v>-0.01573535915653998</v>
+        <v>-0.014078076745719944</v>
       </c>
       <c r="C88">
-        <v>0.011439089652819999</v>
+        <v>0.0078721743345668803</v>
       </c>
       <c r="D88">
-        <v>-0.038155844518409691</v>
+        <v>-0.029507353631004346</v>
       </c>
       <c r="E88">
-        <v>0.006685126205329732</v>
+        <v>0.0013512001395644558</v>
       </c>
     </row>
     <row r="89">
@@ -2061,16 +2061,16 @@
         <v>92</v>
       </c>
       <c r="B89">
-        <v>-0.073389872186703342</v>
+        <v>-0.050234894485538639</v>
       </c>
       <c r="C89">
-        <v>0.0068347181597374403</v>
+        <v>0.0048095076353764686</v>
       </c>
       <c r="D89">
-        <v>-0.086785856152948163</v>
+        <v>-0.059661430013188202</v>
       </c>
       <c r="E89">
-        <v>-0.059993888220458515</v>
+        <v>-0.040808358957889077</v>
       </c>
     </row>
     <row r="90">
@@ -2078,16 +2078,16 @@
         <v>93</v>
       </c>
       <c r="B90">
-        <v>-0.056121709454202896</v>
+        <v>-0.071839226799532321</v>
       </c>
       <c r="C90">
-        <v>0.015002391146914812</v>
+        <v>0.012740333458071809</v>
       </c>
       <c r="D90">
-        <v>-0.085526256439520665</v>
+        <v>-0.096810016967997375</v>
       </c>
       <c r="E90">
-        <v>-0.026717162468885131</v>
+        <v>-0.046868436631067267</v>
       </c>
     </row>
     <row r="91">
@@ -2095,16 +2095,16 @@
         <v>94</v>
       </c>
       <c r="B91">
-        <v>0.035850035039657634</v>
+        <v>0.0066441295074750719</v>
       </c>
       <c r="C91">
-        <v>0.012542513173329181</v>
+        <v>0.0091113710322559723</v>
       </c>
       <c r="D91">
-        <v>0.011266825982682156</v>
+        <v>-0.011213969336032636</v>
       </c>
       <c r="E91">
-        <v>0.060433244096633115</v>
+        <v>0.024502228350982778</v>
       </c>
     </row>
     <row r="92">
@@ -2112,16 +2112,16 @@
         <v>95</v>
       </c>
       <c r="B92">
-        <v>-0.18077088156001245</v>
+        <v>-0.15303979342959115</v>
       </c>
       <c r="C92">
-        <v>0.0045427738328187306</v>
+        <v>0.0033607080662541623</v>
       </c>
       <c r="D92">
-        <v>-0.18967457181360503</v>
+        <v>-0.15962666765613248</v>
       </c>
       <c r="E92">
-        <v>-0.17186719130641986</v>
+        <v>-0.14645291920304981</v>
       </c>
     </row>
     <row r="93">
@@ -2129,16 +2129,16 @@
         <v>96</v>
       </c>
       <c r="B93">
-        <v>-0.037996388240570403</v>
+        <v>-0.054899127714996422</v>
       </c>
       <c r="C93">
-        <v>0.0064448215908199241</v>
+        <v>0.0053199625082072525</v>
       </c>
       <c r="D93">
-        <v>-0.050628030777949654</v>
+        <v>-0.065326074429988584</v>
       </c>
       <c r="E93">
-        <v>-0.025364745703191152</v>
+        <v>-0.04447218100000426</v>
       </c>
     </row>
     <row r="94">
@@ -2146,16 +2146,16 @@
         <v>97</v>
       </c>
       <c r="B94">
-        <v>0.0017724867841721727</v>
+        <v>0.0038543815264766952</v>
       </c>
       <c r="C94">
-        <v>0.0059481475179637327</v>
+        <v>0.0044541030007478749</v>
       </c>
       <c r="D94">
-        <v>-0.0098856905831486604</v>
+        <v>-0.004875509817726646</v>
       </c>
       <c r="E94">
-        <v>0.013430664151493008</v>
+        <v>0.012584272870680036</v>
       </c>
     </row>
     <row r="95">
@@ -2163,16 +2163,16 @@
         <v>98</v>
       </c>
       <c r="B95">
-        <v>-0.099755959046832959</v>
+        <v>-0.078162960113853083</v>
       </c>
       <c r="C95">
-        <v>0.0039269603133101948</v>
+        <v>0.0029519971394014696</v>
       </c>
       <c r="D95">
-        <v>-0.10745267419417436</v>
+        <v>-0.083948774670153783</v>
       </c>
       <c r="E95">
-        <v>-0.092059243899491564</v>
+        <v>-0.072377145557552383</v>
       </c>
     </row>
     <row r="96">
@@ -2180,16 +2180,16 @@
         <v>99</v>
       </c>
       <c r="B96">
-        <v>-0.031072672073093791</v>
+        <v>-0.041691219687175464</v>
       </c>
       <c r="C96">
-        <v>0.0062412691077252903</v>
+        <v>0.0052365874965161529</v>
       </c>
       <c r="D96">
-        <v>-0.043305357572166372</v>
+        <v>-0.051954754078278709</v>
       </c>
       <c r="E96">
-        <v>-0.018839986574021209</v>
+        <v>-0.031427685296072219</v>
       </c>
     </row>
     <row r="97">
@@ -2197,16 +2197,16 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>-0.021184452457021823</v>
+        <v>-0.038160711825125572</v>
       </c>
       <c r="C97">
-        <v>0.0052167082718830859</v>
+        <v>0.0039967230668183119</v>
       </c>
       <c r="D97">
-        <v>-0.031409031870104388</v>
+        <v>-0.045994153866396895</v>
       </c>
       <c r="E97">
-        <v>-0.010959873043939255</v>
+        <v>-0.030327269783854249</v>
       </c>
     </row>
     <row r="98">
@@ -2214,16 +2214,16 @@
         <v>101</v>
       </c>
       <c r="B98">
-        <v>-0.20424173413731866</v>
+        <v>-0.18216586685961245</v>
       </c>
       <c r="C98">
-        <v>0.0054141764979076723</v>
+        <v>0.004232070862710012</v>
       </c>
       <c r="D98">
-        <v>-0.21485334922836619</v>
+        <v>-0.19046058475578651</v>
       </c>
       <c r="E98">
-        <v>-0.19363011904627114</v>
+        <v>-0.17387114896343839</v>
       </c>
     </row>
     <row r="99">
@@ -2231,16 +2231,16 @@
         <v>102</v>
       </c>
       <c r="B99">
-        <v>-0.023389492813110247</v>
+        <v>-0.035737588267795106</v>
       </c>
       <c r="C99">
-        <v>0.0073417840505266233</v>
+        <v>0.0062462736763871712</v>
       </c>
       <c r="D99">
-        <v>-0.037779157881452245</v>
+        <v>-0.047980076574040596</v>
       </c>
       <c r="E99">
-        <v>-0.0089998277447682507</v>
+        <v>-0.023495099961549616</v>
       </c>
     </row>
     <row r="100">
@@ -2248,16 +2248,16 @@
         <v>103</v>
       </c>
       <c r="B100">
-        <v>0.014662601884335134</v>
+        <v>0.019076892869721866</v>
       </c>
       <c r="C100">
-        <v>0.0069270468839173508</v>
+        <v>0.0054392912765237828</v>
       </c>
       <c r="D100">
-        <v>0.0010858085754767884</v>
+        <v>0.0084160631819613259</v>
       </c>
       <c r="E100">
-        <v>0.028239395193193479</v>
+        <v>0.029737722557482405</v>
       </c>
     </row>
     <row r="101">
@@ -2265,16 +2265,16 @@
         <v>104</v>
       </c>
       <c r="B101">
-        <v>-0.12347446503842198</v>
+        <v>-0.10865622928789338</v>
       </c>
       <c r="C101">
-        <v>0.0044203293821019939</v>
+        <v>0.0034496661360710582</v>
       </c>
       <c r="D101">
-        <v>-0.13213817016646631</v>
+        <v>-0.11541745952826349</v>
       </c>
       <c r="E101">
-        <v>-0.11481075991037763</v>
+        <v>-0.10189499904752328</v>
       </c>
     </row>
     <row r="102">
@@ -2282,16 +2282,16 @@
         <v>105</v>
       </c>
       <c r="B102">
-        <v>-0.029319837397206158</v>
+        <v>-0.028633611948908202</v>
       </c>
       <c r="C102">
-        <v>0.0066861846719980678</v>
+        <v>0.0056818351595819558</v>
       </c>
       <c r="D102">
-        <v>-0.042424546893378393</v>
+        <v>-0.039769818812543163</v>
       </c>
       <c r="E102">
-        <v>-0.016215127901033924</v>
+        <v>-0.01749740508527324</v>
       </c>
     </row>
     <row r="103">
@@ -2299,16 +2299,16 @@
         <v>106</v>
       </c>
       <c r="B103">
-        <v>-0.014411996228416598</v>
+        <v>-0.026202341574021709</v>
       </c>
       <c r="C103">
-        <v>0.0057017834910291134</v>
+        <v>0.0045087356811034946</v>
       </c>
       <c r="D103">
-        <v>-0.025587310690330531</v>
+        <v>-0.035039312698315089</v>
       </c>
       <c r="E103">
-        <v>-0.0032366817665026634</v>
+        <v>-0.017365370449728329</v>
       </c>
     </row>
     <row r="104">
@@ -2316,16 +2316,16 @@
         <v>107</v>
       </c>
       <c r="B104">
-        <v>-0.12640464640783272</v>
+        <v>-0.10841170586297924</v>
       </c>
       <c r="C104">
-        <v>0.0065219264729756187</v>
+        <v>0.0041077707013431114</v>
       </c>
       <c r="D104">
-        <v>-0.13918754797224983</v>
+        <v>-0.11646284000186374</v>
       </c>
       <c r="E104">
-        <v>-0.11362174484341561</v>
+        <v>-0.10036057172409474</v>
       </c>
     </row>
     <row r="105">
@@ -2333,16 +2333,16 @@
         <v>108</v>
       </c>
       <c r="B105">
-        <v>-0.069568958483982063</v>
+        <v>-0.063769333156231747</v>
       </c>
       <c r="C105">
-        <v>0.011875256605346742</v>
+        <v>0.0095587325689828855</v>
       </c>
       <c r="D105">
-        <v>-0.092844326102329802</v>
+        <v>-0.082504224586622973</v>
       </c>
       <c r="E105">
-        <v>-0.046293590865634324</v>
+        <v>-0.045034441725840521</v>
       </c>
     </row>
     <row r="106">
@@ -2350,16 +2350,16 @@
         <v>109</v>
       </c>
       <c r="B106">
-        <v>-0.0058822089795355212</v>
+        <v>0.0049746140206533267</v>
       </c>
       <c r="C106">
-        <v>0.010997024638054385</v>
+        <v>0.0072736362732398465</v>
       </c>
       <c r="D106">
-        <v>-0.027436251950152202</v>
+        <v>-0.0092815423159606746</v>
       </c>
       <c r="E106">
-        <v>0.015671833991081158</v>
+        <v>0.019230770357267328</v>
       </c>
     </row>
     <row r="107">
@@ -2367,16 +2367,16 @@
         <v>110</v>
       </c>
       <c r="B107">
-        <v>-0.078294973095662343</v>
+        <v>-0.057994886240499678</v>
       </c>
       <c r="C107">
-        <v>0.0067977313892292656</v>
+        <v>0.0049146167713879649</v>
       </c>
       <c r="D107">
-        <v>-0.091618463336034239</v>
+        <v>-0.067627433501575962</v>
       </c>
       <c r="E107">
-        <v>-0.064971482855290447</v>
+        <v>-0.048362338979423401</v>
       </c>
     </row>
     <row r="108">
@@ -2384,16 +2384,16 @@
         <v>111</v>
       </c>
       <c r="B108">
-        <v>-0.075467540039938552</v>
+        <v>-0.079144436607697377</v>
       </c>
       <c r="C108">
-        <v>0.014589280114758517</v>
+        <v>0.01291205943951285</v>
       </c>
       <c r="D108">
-        <v>-0.10406239324802861</v>
+        <v>-0.10445180614931229</v>
       </c>
       <c r="E108">
-        <v>-0.04687268683184849</v>
+        <v>-0.053837067066082468</v>
       </c>
     </row>
     <row r="109">
@@ -2401,16 +2401,16 @@
         <v>112</v>
       </c>
       <c r="B109">
-        <v>0.074492666262524529</v>
+        <v>0.032747316645117805</v>
       </c>
       <c r="C109">
-        <v>0.012178344761541247</v>
+        <v>0.0091217718189046879</v>
       </c>
       <c r="D109">
-        <v>0.050623223902479156</v>
+        <v>0.014868832474817299</v>
       </c>
       <c r="E109">
-        <v>0.098362108622569902</v>
+        <v>0.050625800815418315</v>
       </c>
     </row>
     <row r="110">
@@ -2418,16 +2418,16 @@
         <v>113</v>
       </c>
       <c r="B110">
-        <v>-0.18267493037322821</v>
+        <v>-0.15030137053954926</v>
       </c>
       <c r="C110">
-        <v>0.0047493738628624129</v>
+        <v>0.0033273949715808713</v>
       </c>
       <c r="D110">
-        <v>-0.19198355002493492</v>
+        <v>-0.15682295222642811</v>
       </c>
       <c r="E110">
-        <v>-0.1733663107215215</v>
+        <v>-0.1437797888526704</v>
       </c>
     </row>
     <row r="111">
@@ -2435,16 +2435,16 @@
         <v>114</v>
       </c>
       <c r="B111">
-        <v>-0.044615853622549904</v>
+        <v>-0.063721199908247025</v>
       </c>
       <c r="C111">
-        <v>0.0067233114934487151</v>
+        <v>0.0053554190800123736</v>
       </c>
       <c r="D111">
-        <v>-0.057793327390585285</v>
+        <v>-0.074217640305636004</v>
       </c>
       <c r="E111">
-        <v>-0.031438379854514524</v>
+        <v>-0.053224759510858054</v>
       </c>
     </row>
     <row r="112">
@@ -2452,16 +2452,16 @@
         <v>115</v>
       </c>
       <c r="B112">
-        <v>0.029848286824122095</v>
+        <v>0.028675356077107979</v>
       </c>
       <c r="C112">
-        <v>0.0061190126055906454</v>
+        <v>0.004339658526389574</v>
       </c>
       <c r="D112">
-        <v>0.017855219393731796</v>
+        <v>0.020169772034717072</v>
       </c>
       <c r="E112">
-        <v>0.041841354254512395</v>
+        <v>0.037180940119498886</v>
       </c>
     </row>
     <row r="113">
@@ -2469,16 +2469,16 @@
         <v>116</v>
       </c>
       <c r="B113">
-        <v>-0.10597990883778588</v>
+        <v>-0.084063785111363226</v>
       </c>
       <c r="C113">
-        <v>0.0042350981194045588</v>
+        <v>0.0031934451690524548</v>
       </c>
       <c r="D113">
-        <v>-0.1142805641144931</v>
+        <v>-0.090322829639976177</v>
       </c>
       <c r="E113">
-        <v>-0.097679253561078663</v>
+        <v>-0.077804740582750276</v>
       </c>
     </row>
     <row r="114">
@@ -2486,16 +2486,16 @@
         <v>117</v>
       </c>
       <c r="B114">
-        <v>-0.036990325284355384</v>
+        <v>-0.050952662400742303</v>
       </c>
       <c r="C114">
-        <v>0.0066536940652216344</v>
+        <v>0.0056542845404010268</v>
       </c>
       <c r="D114">
-        <v>-0.05003135035506677</v>
+        <v>-0.062034868871291698</v>
       </c>
       <c r="E114">
-        <v>-0.023949300213643998</v>
+        <v>-0.039870455930192908</v>
       </c>
     </row>
     <row r="115">
@@ -2503,16 +2503,16 @@
         <v>118</v>
       </c>
       <c r="B115">
-        <v>0.00031830769003438557</v>
+        <v>-0.016215328338629636</v>
       </c>
       <c r="C115">
-        <v>0.0055271534461004352</v>
+        <v>0.0042596437704718552</v>
       </c>
       <c r="D115">
-        <v>-0.010514734219274322</v>
+        <v>-0.024564086067049601</v>
       </c>
       <c r="E115">
-        <v>0.011151349599343094</v>
+        <v>-0.0078665706102096708</v>
       </c>
     </row>
     <row r="116">
@@ -2520,16 +2520,16 @@
         <v>119</v>
       </c>
       <c r="B116">
-        <v>-0.20697300060836446</v>
+        <v>-0.17384839226280152</v>
       </c>
       <c r="C116">
-        <v>0.0057855737005392998</v>
+        <v>0.0042958262262103508</v>
       </c>
       <c r="D116">
-        <v>-0.21831254249709611</v>
+        <v>-0.18226806854737665</v>
       </c>
       <c r="E116">
-        <v>-0.19563345871963281</v>
+        <v>-0.16542871597822639</v>
       </c>
     </row>
     <row r="117">
@@ -2537,16 +2537,16 @@
         <v>120</v>
       </c>
       <c r="B117">
-        <v>-0.031888508393979921</v>
+        <v>-0.055896913775923533</v>
       </c>
       <c r="C117">
-        <v>0.0079563858852960585</v>
+        <v>0.0064940623742946726</v>
       </c>
       <c r="D117">
-        <v>-0.047482773664650979</v>
+        <v>-0.068625059674794237</v>
       </c>
       <c r="E117">
-        <v>-0.016294243123308863</v>
+        <v>-0.043168767877052837</v>
       </c>
     </row>
     <row r="118">
@@ -2554,16 +2554,16 @@
         <v>121</v>
       </c>
       <c r="B118">
-        <v>0.044291654679563093</v>
+        <v>0.037913473163288282</v>
       </c>
       <c r="C118">
-        <v>0.0073394865611155664</v>
+        <v>0.0054479115546837084</v>
       </c>
       <c r="D118">
-        <v>0.029906492617969273</v>
+        <v>0.027235748017525568</v>
       </c>
       <c r="E118">
-        <v>0.058676816741156913</v>
+        <v>0.048591198309050995</v>
       </c>
     </row>
     <row r="119">
@@ -2571,16 +2571,16 @@
         <v>122</v>
       </c>
       <c r="B119">
-        <v>-0.12973727220609915</v>
+        <v>-0.10784364943422567</v>
       </c>
       <c r="C119">
-        <v>0.0049312251690260536</v>
+        <v>0.003637720850072934</v>
       </c>
       <c r="D119">
-        <v>-0.13940231684223359</v>
+        <v>-0.114973460623882</v>
       </c>
       <c r="E119">
-        <v>-0.12007222756996472</v>
+        <v>-0.10071383824456934</v>
       </c>
     </row>
     <row r="120">
@@ -2588,16 +2588,16 @@
         <v>123</v>
       </c>
       <c r="B120">
-        <v>-0.028308135089085341</v>
+        <v>-0.041437911980564714</v>
       </c>
       <c r="C120">
-        <v>0.0074464776003906278</v>
+        <v>0.0060420022515361585</v>
       </c>
       <c r="D120">
-        <v>-0.042902994565754769</v>
+        <v>-0.053280034297363041</v>
       </c>
       <c r="E120">
-        <v>-0.013713275612415914</v>
+        <v>-0.029595789663766386</v>
       </c>
     </row>
     <row r="121">
@@ -2605,16 +2605,16 @@
         <v>124</v>
       </c>
       <c r="B121">
-        <v>0.003263927099746418</v>
+        <v>-0.0094000162365263096</v>
       </c>
       <c r="C121">
-        <v>0.0062913244014474543</v>
+        <v>0.0047082473615943556</v>
       </c>
       <c r="D121">
-        <v>-0.0090668688132702607</v>
+        <v>-0.018628023581205418</v>
       </c>
       <c r="E121">
-        <v>0.015594723012763096</v>
+        <v>-0.00017200889184720326</v>
       </c>
     </row>
     <row r="122">
@@ -2622,16 +2622,16 @@
         <v>125</v>
       </c>
       <c r="B122">
-        <v>-0.12538890473117439</v>
+        <v>-0.11360634552211442</v>
       </c>
       <c r="C122">
-        <v>0.0066294523941429935</v>
+        <v>0.0043205750612752307</v>
       </c>
       <c r="D122">
-        <v>-0.13838255587573492</v>
+        <v>-0.12207457121058146</v>
       </c>
       <c r="E122">
-        <v>-0.11239525358661387</v>
+        <v>-0.10513811983364738</v>
       </c>
     </row>
     <row r="123">
@@ -2639,16 +2639,16 @@
         <v>126</v>
       </c>
       <c r="B123">
-        <v>-0.068421513503536438</v>
+        <v>-0.075956331548065512</v>
       </c>
       <c r="C123">
-        <v>0.011846882433903153</v>
+        <v>0.010041080936780104</v>
       </c>
       <c r="D123">
-        <v>-0.091641268069201323</v>
+        <v>-0.095636614455526681</v>
       </c>
       <c r="E123">
-        <v>-0.045201758937871553</v>
+        <v>-0.056276048640604343</v>
       </c>
     </row>
     <row r="124">
@@ -2656,16 +2656,16 @@
         <v>127</v>
       </c>
       <c r="B124">
-        <v>0.021472322387155698</v>
+        <v>0.02754047524218893</v>
       </c>
       <c r="C124">
-        <v>0.010859199607261338</v>
+        <v>0.0074497595922980017</v>
       </c>
       <c r="D124">
-        <v>0.00018841490626594209</v>
+        <v>0.012939121334965858</v>
       </c>
       <c r="E124">
-        <v>0.042756229868045455</v>
+        <v>0.042141829149412002</v>
       </c>
     </row>
     <row r="125">
@@ -2673,16 +2673,16 @@
         <v>128</v>
       </c>
       <c r="B125">
-        <v>-0.091899972028656018</v>
+        <v>-0.061345753639363329</v>
       </c>
       <c r="C125">
-        <v>0.007309597104717222</v>
+        <v>0.0050979623257709538</v>
       </c>
       <c r="D125">
-        <v>-0.10622671430624295</v>
+        <v>-0.071337654396318312</v>
       </c>
       <c r="E125">
-        <v>-0.077573229751069089</v>
+        <v>-0.051353852882408346</v>
       </c>
     </row>
     <row r="126">
@@ -2690,16 +2690,16 @@
         <v>129</v>
       </c>
       <c r="B126">
-        <v>-0.086166796136866064</v>
+        <v>-0.091242892256369543</v>
       </c>
       <c r="C126">
-        <v>0.015293324397220701</v>
+        <v>0.013096250749625542</v>
       </c>
       <c r="D126">
-        <v>-0.11614156958438149</v>
+        <v>-0.11691127295760717</v>
       </c>
       <c r="E126">
-        <v>-0.05619202268935064</v>
+        <v>-0.065574511555131915</v>
       </c>
     </row>
     <row r="127">
@@ -2707,16 +2707,16 @@
         <v>130</v>
       </c>
       <c r="B127">
-        <v>0.10034342776062877</v>
+        <v>0.064425789813945714</v>
       </c>
       <c r="C127">
-        <v>0.012583392676954056</v>
+        <v>0.0091667911245304629</v>
       </c>
       <c r="D127">
-        <v>0.075680095257110488</v>
+        <v>0.0464590687354033</v>
       </c>
       <c r="E127">
-        <v>0.12500676026414706</v>
+        <v>0.082392510892488127</v>
       </c>
     </row>
     <row r="128">
@@ -2724,16 +2724,16 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>-0.17922925645424539</v>
+        <v>-0.14948682209205238</v>
       </c>
       <c r="C128">
-        <v>0.0049871830957619557</v>
+        <v>0.0036165202640044609</v>
       </c>
       <c r="D128">
-        <v>-0.18900397453548104</v>
+        <v>-0.15657507958038783</v>
       </c>
       <c r="E128">
-        <v>-0.16945453837300975</v>
+        <v>-0.14239856460371694</v>
       </c>
     </row>
     <row r="129">
@@ -2741,16 +2741,16 @@
         <v>132</v>
       </c>
       <c r="B129">
-        <v>-0.043607715354031774</v>
+        <v>-0.068736299220748392</v>
       </c>
       <c r="C129">
-        <v>0.0071075090492879545</v>
+        <v>0.0059968330340104256</v>
       </c>
       <c r="D129">
-        <v>-0.057538203945007922</v>
+        <v>-0.080489889289826283</v>
       </c>
       <c r="E129">
-        <v>-0.029677226763055627</v>
+        <v>-0.056982709151670495</v>
       </c>
     </row>
     <row r="130">
@@ -2758,16 +2758,16 @@
         <v>133</v>
       </c>
       <c r="B130">
-        <v>0.058427523266053397</v>
+        <v>0.052229269736044054</v>
       </c>
       <c r="C130">
-        <v>0.0063745415663229235</v>
+        <v>0.0046722307585032137</v>
       </c>
       <c r="D130">
-        <v>0.045933627310864859</v>
+        <v>0.043071855358799246</v>
       </c>
       <c r="E130">
-        <v>0.070921419221241927</v>
+        <v>0.061386684113288861</v>
       </c>
     </row>
     <row r="131">
@@ -2775,16 +2775,16 @@
         <v>134</v>
       </c>
       <c r="B131">
-        <v>-0.11101824164294564</v>
+        <v>-0.083493386186789795</v>
       </c>
       <c r="C131">
-        <v>0.0047570374174150405</v>
+        <v>0.0034996055969884082</v>
       </c>
       <c r="D131">
-        <v>-0.12034188105508553</v>
+        <v>-0.090352494799771824</v>
       </c>
       <c r="E131">
-        <v>-0.10169460223080576</v>
+        <v>-0.076634277573807766</v>
       </c>
     </row>
     <row r="132">
@@ -2792,16 +2792,16 @@
         <v>135</v>
       </c>
       <c r="B132">
-        <v>-0.045525095479656698</v>
+        <v>-0.068309900862705164</v>
       </c>
       <c r="C132">
-        <v>0.0073411687232049225</v>
+        <v>0.0061409346860698934</v>
       </c>
       <c r="D132">
-        <v>-0.059913548635031628</v>
+        <v>-0.080345925160194481</v>
       </c>
       <c r="E132">
-        <v>-0.031136642324281767</v>
+        <v>-0.056273876565215847</v>
       </c>
     </row>
     <row r="133">
@@ -2809,16 +2809,16 @@
         <v>136</v>
       </c>
       <c r="B133">
-        <v>0.024080054530001775</v>
+        <v>0.0078269668440447207</v>
       </c>
       <c r="C133">
-        <v>0.0060721617265666068</v>
+        <v>0.0045594052843683733</v>
       </c>
       <c r="D133">
-        <v>0.012178814026102604</v>
+        <v>-0.0011093133136391344</v>
       </c>
       <c r="E133">
-        <v>0.035981295033900948</v>
+        <v>0.016763247001728578</v>
       </c>
     </row>
     <row r="134">
@@ -2826,16 +2826,16 @@
         <v>137</v>
       </c>
       <c r="B134">
-        <v>-0.20009145815180684</v>
+        <v>-0.16226157223923607</v>
       </c>
       <c r="C134">
-        <v>0.006094471200048965</v>
+        <v>0.0046087968618687379</v>
       </c>
       <c r="D134">
-        <v>-0.21203642939228762</v>
+        <v>-0.17129466054284109</v>
       </c>
       <c r="E134">
-        <v>-0.18814648691132607</v>
+        <v>-0.15322848393563104</v>
       </c>
     </row>
     <row r="135">
@@ -2843,16 +2843,16 @@
         <v>138</v>
       </c>
       <c r="B135">
-        <v>-0.037472498273489252</v>
+        <v>-0.067171958875570301</v>
       </c>
       <c r="C135">
-        <v>0.00842024136113299</v>
+        <v>0.0071353783116575205</v>
       </c>
       <c r="D135">
-        <v>-0.053975905639797275</v>
+        <v>-0.081157062645732136</v>
       </c>
       <c r="E135">
-        <v>-0.020969090907181225</v>
+        <v>-0.053186855105408458</v>
       </c>
     </row>
     <row r="136">
@@ -2860,16 +2860,16 @@
         <v>139</v>
       </c>
       <c r="B136">
-        <v>0.074828441885253838</v>
+        <v>0.060282868849169467</v>
       </c>
       <c r="C136">
-        <v>0.0076285430525930608</v>
+        <v>0.0057633739743206463</v>
       </c>
       <c r="D136">
-        <v>0.059876738221569061</v>
+        <v>0.04898684787079461</v>
       </c>
       <c r="E136">
-        <v>0.089780145548938622</v>
+        <v>0.071578889827544318</v>
       </c>
     </row>
     <row r="137">
@@ -2877,16 +2877,16 @@
         <v>140</v>
       </c>
       <c r="B137">
-        <v>-0.12242651842613297</v>
+        <v>-0.10260903367150272</v>
       </c>
       <c r="C137">
-        <v>0.0055656558555464844</v>
+        <v>0.0041250659733125484</v>
       </c>
       <c r="D137">
-        <v>-0.13333502704810776</v>
+        <v>-0.11069402500172112</v>
       </c>
       <c r="E137">
-        <v>-0.11151800980415819</v>
+        <v>-0.094524042341284309</v>
       </c>
     </row>
     <row r="138">
@@ -2894,16 +2894,16 @@
         <v>141</v>
       </c>
       <c r="B138">
-        <v>-0.037454395270240047</v>
+        <v>-0.058326230484136696</v>
       </c>
       <c r="C138">
-        <v>0.0082873318066447495</v>
+        <v>0.0068619889797527219</v>
       </c>
       <c r="D138">
-        <v>-0.053697302272091255</v>
+        <v>-0.071775499360872658</v>
       </c>
       <c r="E138">
-        <v>-0.021211488268388839</v>
+        <v>-0.044876961607400727</v>
       </c>
     </row>
     <row r="139">
@@ -2911,16 +2911,16 @@
         <v>142</v>
       </c>
       <c r="B139">
-        <v>0.018506899897803738</v>
+        <v>0.0060281385853554687</v>
       </c>
       <c r="C139">
-        <v>0.0069701073608765879</v>
+        <v>0.0052399107014338394</v>
       </c>
       <c r="D139">
-        <v>0.0048457109533883852</v>
+        <v>-0.0042419111220413841</v>
       </c>
       <c r="E139">
-        <v>0.032168088842219091</v>
+        <v>0.016298188292752321</v>
       </c>
     </row>
     <row r="140">
@@ -2928,16 +2928,16 @@
         <v>143</v>
       </c>
       <c r="B140">
-        <v>-0.11951360740113488</v>
+        <v>-0.11079374089759307</v>
       </c>
       <c r="C140">
-        <v>0.0072185466818314023</v>
+        <v>0.0048353825065080742</v>
       </c>
       <c r="D140">
-        <v>-0.13366187663635992</v>
+        <v>-0.12027097709288095</v>
       </c>
       <c r="E140">
-        <v>-0.10536533816590986</v>
+        <v>-0.10131650470230519</v>
       </c>
     </row>
     <row r="141">
@@ -2945,16 +2945,16 @@
         <v>144</v>
       </c>
       <c r="B141">
-        <v>-0.058748964926760891</v>
+        <v>-0.074288220901758947</v>
       </c>
       <c r="C141">
-        <v>0.012690396874412726</v>
+        <v>0.011234096546225805</v>
       </c>
       <c r="D141">
-        <v>-0.083621998183296797</v>
+        <v>-0.096306786395998836</v>
       </c>
       <c r="E141">
-        <v>-0.033875931670224978</v>
+        <v>-0.052269655407519058</v>
       </c>
     </row>
     <row r="142">
@@ -2962,16 +2962,16 @@
         <v>145</v>
       </c>
       <c r="B142">
-        <v>0.03928518867451819</v>
+        <v>0.03694272435267959</v>
       </c>
       <c r="C142">
-        <v>0.011502687988613513</v>
+        <v>0.0080445726448871418</v>
       </c>
       <c r="D142">
-        <v>0.016740051299247546</v>
+        <v>0.021175550826462525</v>
       </c>
       <c r="E142">
-        <v>0.061830326049788831</v>
+        <v>0.052709897878896655</v>
       </c>
     </row>
     <row r="143">
@@ -2979,16 +2979,16 @@
         <v>146</v>
       </c>
       <c r="B143">
-        <v>-0.086952508384541702</v>
+        <v>-0.064493498031780366</v>
       </c>
       <c r="C143">
-        <v>0.0082157460532521227</v>
+        <v>0.0058529120540440592</v>
       </c>
       <c r="D143">
-        <v>-0.10305529416559175</v>
+        <v>-0.075965084647389519</v>
       </c>
       <c r="E143">
-        <v>-0.070849722603491649</v>
+        <v>-0.053021911416171214</v>
       </c>
     </row>
     <row r="144">
@@ -2996,16 +2996,16 @@
         <v>147</v>
       </c>
       <c r="B144">
-        <v>-0.082260562776086746</v>
+        <v>-0.11478585904035545</v>
       </c>
       <c r="C144">
-        <v>0.015969336716361089</v>
+        <v>0.014141490275390111</v>
       </c>
       <c r="D144">
-        <v>-0.11356031407587641</v>
+        <v>-0.14250288760152147</v>
       </c>
       <c r="E144">
-        <v>-0.050960811476297087</v>
+        <v>-0.08706883047918941</v>
       </c>
     </row>
     <row r="145">
@@ -3013,16 +3013,16 @@
         <v>148</v>
       </c>
       <c r="B145">
-        <v>0.089361972717976607</v>
+        <v>0.06941433137136041</v>
       </c>
       <c r="C145">
-        <v>0.013099570195236776</v>
+        <v>0.0097965936635965468</v>
       </c>
       <c r="D145">
-        <v>0.063686937083905687</v>
+        <v>0.050213210337562361</v>
       </c>
       <c r="E145">
-        <v>0.11503700835204753</v>
+        <v>0.08861545240515846</v>
       </c>
     </row>
     <row r="146">
@@ -3030,16 +3030,16 @@
         <v>149</v>
       </c>
       <c r="B146">
-        <v>-0.14943134475776654</v>
+        <v>-0.13834770749091596</v>
       </c>
       <c r="C146">
-        <v>0.0052584794175212658</v>
+        <v>0.0040893426117577826</v>
       </c>
       <c r="D146">
-        <v>-0.15973779488307471</v>
+        <v>-0.14636268080066472</v>
       </c>
       <c r="E146">
-        <v>-0.13912489463245836</v>
+        <v>-0.1303327341811672</v>
       </c>
     </row>
     <row r="147">
@@ -3047,16 +3047,16 @@
         <v>150</v>
       </c>
       <c r="B147">
-        <v>-0.029229117315318635</v>
+        <v>-0.076722724093914549</v>
       </c>
       <c r="C147">
-        <v>0.0074858432829302988</v>
+        <v>0.0071290842902312478</v>
       </c>
       <c r="D147">
-        <v>-0.043901128806762751</v>
+        <v>-0.090695488357995541</v>
       </c>
       <c r="E147">
-        <v>-0.014557105823874514</v>
+        <v>-0.062749959829833557</v>
       </c>
     </row>
     <row r="148">
@@ -3064,16 +3064,16 @@
         <v>151</v>
       </c>
       <c r="B148">
-        <v>0.066942331815350919</v>
+        <v>0.067937285421854621</v>
       </c>
       <c r="C148">
-        <v>0.0066793554134627038</v>
+        <v>0.0052979243294091483</v>
       </c>
       <c r="D148">
-        <v>0.053851010546946965</v>
+        <v>0.0575535327924728</v>
       </c>
       <c r="E148">
-        <v>0.080033653083754874</v>
+        <v>0.078321038051236441</v>
       </c>
     </row>
     <row r="149">
@@ -3081,16 +3081,16 @@
         <v>152</v>
       </c>
       <c r="B149">
-        <v>-0.10872749551982962</v>
+        <v>-0.078858626048711064</v>
       </c>
       <c r="C149">
-        <v>0.0059195812784394349</v>
+        <v>0.0044869944218723949</v>
       </c>
       <c r="D149">
-        <v>-0.12032968328252637</v>
+        <v>-0.087652983364847559</v>
       </c>
       <c r="E149">
-        <v>-0.097125307757132864</v>
+        <v>-0.070064268732574569</v>
       </c>
     </row>
     <row r="150">
@@ -3098,16 +3098,16 @@
         <v>153</v>
       </c>
       <c r="B150">
-        <v>-0.056697703952124381</v>
+        <v>-0.091594231155160452</v>
       </c>
       <c r="C150">
-        <v>0.0086309812520962408</v>
+        <v>0.0076896154901570602</v>
       </c>
       <c r="D150">
-        <v>-0.073614147928975276</v>
+        <v>-0.10666561745207492</v>
       </c>
       <c r="E150">
-        <v>-0.039781259975273493</v>
+        <v>-0.076522844858245981</v>
       </c>
     </row>
     <row r="151">
@@ -3115,16 +3115,16 @@
         <v>154</v>
       </c>
       <c r="B151">
-        <v>0.047132497943722367</v>
+        <v>0.025286418786274096</v>
       </c>
       <c r="C151">
-        <v>0.0073027848518367813</v>
+        <v>0.0056294766509290637</v>
       </c>
       <c r="D151">
-        <v>0.032819275934221619</v>
+        <v>0.014252834940083711</v>
       </c>
       <c r="E151">
-        <v>0.061445719953223114</v>
+        <v>0.036320002632464481</v>
       </c>
     </row>
     <row r="152">
@@ -3132,16 +3132,16 @@
         <v>155</v>
       </c>
       <c r="B152">
-        <v>-0.1604055052210851</v>
+        <v>-0.14435422791117641</v>
       </c>
       <c r="C152">
-        <v>0.0060587131552550339</v>
+        <v>0.0048673213628476573</v>
       </c>
       <c r="D152">
-        <v>-0.17228039182211824</v>
+        <v>-0.15389401562375499</v>
       </c>
       <c r="E152">
-        <v>-0.14853061862005196</v>
+        <v>-0.13481444019859784</v>
       </c>
     </row>
     <row r="153">
@@ -3149,16 +3149,16 @@
         <v>156</v>
       </c>
       <c r="B153">
-        <v>-0.022215854478820001</v>
+        <v>-0.066356561352776372</v>
       </c>
       <c r="C153">
-        <v>0.0082795884051694701</v>
+        <v>0.0077648835612637171</v>
       </c>
       <c r="D153">
-        <v>-0.038443586489756862</v>
+        <v>-0.081575474439708584</v>
       </c>
       <c r="E153">
-        <v>-0.0059881224678831439</v>
+        <v>-0.05113764826584416</v>
       </c>
     </row>
     <row r="154">
@@ -3166,16 +3166,16 @@
         <v>157</v>
       </c>
       <c r="B154">
-        <v>0.082796617868243078</v>
+        <v>0.08313908617479962</v>
       </c>
       <c r="C154">
-        <v>0.0074428971785316274</v>
+        <v>0.0060151594276179029</v>
       </c>
       <c r="D154">
-        <v>0.068208774259645596</v>
+        <v>0.071349574096390658</v>
       </c>
       <c r="E154">
-        <v>0.097384461476840559</v>
+        <v>0.094928598253208582</v>
       </c>
     </row>
     <row r="155">
@@ -3183,16 +3183,16 @@
         <v>158</v>
       </c>
       <c r="B155">
-        <v>-0.11569384366322789</v>
+        <v>-0.093298755270002573</v>
       </c>
       <c r="C155">
-        <v>0.0069130637027892405</v>
+        <v>0.0052316345685546051</v>
       </c>
       <c r="D155">
-        <v>-0.12924322885041764</v>
+        <v>-0.10355258403378077</v>
       </c>
       <c r="E155">
-        <v>-0.10214445847603815</v>
+        <v>-0.083044926506224373</v>
       </c>
     </row>
     <row r="156">
@@ -3200,16 +3200,16 @@
         <v>159</v>
       </c>
       <c r="B156">
-        <v>-0.054761474725207857</v>
+        <v>-0.08412572301073902</v>
       </c>
       <c r="C156">
-        <v>0.0098463667445633819</v>
+        <v>0.0086547932775020153</v>
       </c>
       <c r="D156">
-        <v>-0.074060040665312882</v>
+        <v>-0.10108882834435996</v>
       </c>
       <c r="E156">
-        <v>-0.035462908785102831</v>
+        <v>-0.067162617677118078</v>
       </c>
     </row>
     <row r="157">
@@ -3217,16 +3217,16 @@
         <v>160</v>
       </c>
       <c r="B157">
-        <v>0.043787948293691467</v>
+        <v>0.0251054788508982</v>
       </c>
       <c r="C157">
-        <v>0.0084393771315502825</v>
+        <v>0.0064684389672375348</v>
       </c>
       <c r="D157">
-        <v>0.027247037286434485</v>
+        <v>0.012427554835014848</v>
       </c>
       <c r="E157">
-        <v>0.060328859300948445</v>
+        <v>0.03778340286678155</v>
       </c>
     </row>
     <row r="158">
@@ -3234,16 +3234,16 @@
         <v>161</v>
       </c>
       <c r="B158">
-        <v>-0.1228533372510533</v>
+        <v>-0.11540147864260129</v>
       </c>
       <c r="C158">
-        <v>0.0093874452994774267</v>
+        <v>0.0064902794555746325</v>
       </c>
       <c r="D158">
-        <v>-0.14125262306051456</v>
+        <v>-0.12812227400700471</v>
       </c>
       <c r="E158">
-        <v>-0.10445405144159202</v>
+        <v>-0.10268068327819788</v>
       </c>
     </row>
     <row r="159">
@@ -3251,16 +3251,16 @@
         <v>162</v>
       </c>
       <c r="B159">
-        <v>-0.046950936311578637</v>
+        <v>-0.082530276505072248</v>
       </c>
       <c r="C159">
-        <v>0.015747005619895928</v>
+        <v>0.014975011866144137</v>
       </c>
       <c r="D159">
-        <v>-0.077814887876738403</v>
+        <v>-0.11188094820305487</v>
       </c>
       <c r="E159">
-        <v>-0.016086984746418866</v>
+        <v>-0.053179604807089623</v>
       </c>
     </row>
     <row r="160">
@@ -3268,16 +3268,16 @@
         <v>163</v>
       </c>
       <c r="B160">
-        <v>0.044628433442431337</v>
+        <v>0.0428155851412668</v>
       </c>
       <c r="C160">
-        <v>0.014828368224713057</v>
+        <v>0.010577891061798912</v>
       </c>
       <c r="D160">
-        <v>0.015565000703215572</v>
+        <v>0.022083166991148425</v>
       </c>
       <c r="E160">
-        <v>0.073691866181647109</v>
+        <v>0.063548003291385172</v>
       </c>
     </row>
     <row r="161">
@@ -3285,16 +3285,16 @@
         <v>164</v>
       </c>
       <c r="B161">
-        <v>-0.088622726985119402</v>
+        <v>-0.070159197922018843</v>
       </c>
       <c r="C161">
-        <v>0.010807867844891286</v>
+        <v>0.0078250852147290269</v>
       </c>
       <c r="D161">
-        <v>-0.10980604734679157</v>
+        <v>-0.085496203157432005</v>
       </c>
       <c r="E161">
-        <v>-0.067439406623447232</v>
+        <v>-0.054822192686605681</v>
       </c>
     </row>
     <row r="162">
@@ -3302,16 +3302,16 @@
         <v>165</v>
       </c>
       <c r="B162">
-        <v>-0.096857891285891243</v>
+        <v>-0.13357109414354879</v>
       </c>
       <c r="C162">
-        <v>0.018768403829266395</v>
+        <v>0.017363830708986415</v>
       </c>
       <c r="D162">
-        <v>-0.13364378806945651</v>
+        <v>-0.16760384333192607</v>
       </c>
       <c r="E162">
-        <v>-0.060071994502325983</v>
+        <v>-0.099538344955171484</v>
       </c>
     </row>
     <row r="163">
@@ -3319,16 +3319,16 @@
         <v>166</v>
       </c>
       <c r="B163">
-        <v>0.09445641664193534</v>
+        <v>0.075107596682770603</v>
       </c>
       <c r="C163">
-        <v>0.015623448440812723</v>
+        <v>0.011985000039214896</v>
       </c>
       <c r="D163">
-        <v>0.063834603142222571</v>
+        <v>0.051617244398571085</v>
       </c>
       <c r="E163">
-        <v>0.12507823014164809</v>
+        <v>0.09859794896697012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>